<commit_message>
Add in all examples for Text Functions
</commit_message>
<xml_diff>
--- a/2_Formulas_and_Functions/7_Text_Functions/1_Text_Formatting_and_Combination.xlsx
+++ b/2_Formulas_and_Functions/7_Text_Functions/1_Text_Formatting_and_Combination.xlsx
@@ -8,24 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_and_Functions\7_Text_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4D5641-38E6-40C8-B351-52B43F3AA558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81640F0-5F8A-4A7A-981C-BB93D4EAF48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="TEXTJOIN" sheetId="3" r:id="rId2"/>
+    <sheet name="UPPER_LOWER" sheetId="4" r:id="rId3"/>
+    <sheet name="TRIM" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="76">
   <si>
     <t>job_title_short</t>
   </si>
@@ -54,9 +68,6 @@
     <t>job_work_from_home</t>
   </si>
   <si>
-    <t>job_skills</t>
-  </si>
-  <si>
     <t>Senior Data Engineer</t>
   </si>
   <si>
@@ -75,9 +86,6 @@
     <t>Full-time</t>
   </si>
   <si>
-    <t>['sql', 'python', 'gcp', 'power bi', 'tableau']</t>
-  </si>
-  <si>
     <t>Data Analyst</t>
   </si>
   <si>
@@ -96,9 +104,6 @@
     <t>Contractor</t>
   </si>
   <si>
-    <t>['sql', 'r', 'python', 'hadoop', 'spark', 'looker']</t>
-  </si>
-  <si>
     <t>Reston, VA</t>
   </si>
   <si>
@@ -108,9 +113,6 @@
     <t>via Snagajob</t>
   </si>
   <si>
-    <t>['sql', 'power bi']</t>
-  </si>
-  <si>
     <t>Data Scientist</t>
   </si>
   <si>
@@ -120,9 +122,6 @@
     <t>Apple</t>
   </si>
   <si>
-    <t>['sql', 'python', 'r']</t>
-  </si>
-  <si>
     <t>Senior Data Analyst</t>
   </si>
   <si>
@@ -135,9 +134,6 @@
     <t>Securian Financial Group</t>
   </si>
   <si>
-    <t>['sql', 'aws', 'tableau', 'flow']</t>
-  </si>
-  <si>
     <t>Des Moines, IA</t>
   </si>
   <si>
@@ -147,18 +143,12 @@
     <t>Full-time and Part-time</t>
   </si>
   <si>
-    <t>['r', 'python', 'sql', 'hadoop']</t>
-  </si>
-  <si>
     <t>Atlanta, GA</t>
   </si>
   <si>
     <t>The E Group</t>
   </si>
   <si>
-    <t>['sql', 'python', 'r', 'sql server', 'mysql', 'oracle', 'spss']</t>
-  </si>
-  <si>
     <t>Jacksonville, FL</t>
   </si>
   <si>
@@ -168,18 +158,12 @@
     <t>via Indeed</t>
   </si>
   <si>
-    <t>['power bi']</t>
-  </si>
-  <si>
     <t>Dublin, CA</t>
   </si>
   <si>
     <t>NextPhase</t>
   </si>
   <si>
-    <t>['sql', 'python', 'r', 'snowflake', 'oracle', 'tableau']</t>
-  </si>
-  <si>
     <t>Charlotte, NC</t>
   </si>
   <si>
@@ -189,18 +173,12 @@
     <t>via LinkedIn</t>
   </si>
   <si>
-    <t>['sql', 'python', 'r', 'power bi']</t>
-  </si>
-  <si>
     <t>Sunnyvale, CA</t>
   </si>
   <si>
     <t>Walmart</t>
   </si>
   <si>
-    <t>['python', 'scala', 'r', 'spark', 'tensorflow']</t>
-  </si>
-  <si>
     <t>Senior Data Scientist</t>
   </si>
   <si>
@@ -210,9 +188,6 @@
     <t>Harnham</t>
   </si>
   <si>
-    <t>['python', 'sql', 'git']</t>
-  </si>
-  <si>
     <t>Houston, TX</t>
   </si>
   <si>
@@ -222,9 +197,6 @@
     <t>via IT JobServe</t>
   </si>
   <si>
-    <t>['python', 'sql', 'spark']</t>
-  </si>
-  <si>
     <t>Johannesburg, South Africa</t>
   </si>
   <si>
@@ -237,9 +209,6 @@
     <t>via Ai-Jobs.net</t>
   </si>
   <si>
-    <t>['sql', 'python', 'c#', 'java', 'c++', 'html', 'sas', 'sas', 'r', 'tableau', 'power bi', 'spss', 'qlik']</t>
-  </si>
-  <si>
     <t>Data Engineer</t>
   </si>
   <si>
@@ -252,9 +221,6 @@
     <t>Vattenfall</t>
   </si>
   <si>
-    <t>['python', 'azure']</t>
-  </si>
-  <si>
     <t>Amsterdam, Netherlands</t>
   </si>
   <si>
@@ -264,9 +230,6 @@
     <t>Devoteam</t>
   </si>
   <si>
-    <t>['sql', 'gcp', 'unix', 'docker']</t>
-  </si>
-  <si>
     <t>Business Analyst</t>
   </si>
   <si>
@@ -276,24 +239,15 @@
     <t>DISYS</t>
   </si>
   <si>
-    <t>['sql', 'html', 'sql server', 'oracle', 'snowflake', 'power bi', 'sharepoint', 'dax', 'excel', 'jira']</t>
-  </si>
-  <si>
     <t>Broomfield, CO</t>
   </si>
   <si>
     <t>Datalab USA</t>
   </si>
   <si>
-    <t>['sql', 'r', 'python', 'tableau', 'excel']</t>
-  </si>
-  <si>
     <t>Fortira Inc.</t>
   </si>
   <si>
-    <t>['sql', 'sas', 'sas', 'r', 'python', 'snowflake', 'hadoop']</t>
-  </si>
-  <si>
     <t>Palo Alto, CA</t>
   </si>
   <si>
@@ -303,7 +257,16 @@
     <t>via Ladders</t>
   </si>
   <si>
-    <t>['power bi', 'excel', 'powerpoint', 'flow']</t>
+    <t>TEXTJOIN</t>
+  </si>
+  <si>
+    <t>UPPER</t>
+  </si>
+  <si>
+    <t>LOWER</t>
+  </si>
+  <si>
+    <t>TRIM</t>
   </si>
 </sst>
 </file>
@@ -327,15 +290,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -358,16 +327,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +648,618 @@
     <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="80.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44996.547291666669</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>135000</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45097.915243055562</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>35000</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45173.250416666669</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45156.253321759257</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45147.802951388891</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45202.753101851849</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44949.850462962961</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45001.627175925933</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>115000</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45041.375868055547</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45106.587094907409</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>105000</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45029.919687499998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>195000</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45091.502789351849</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>165000</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45175.543124999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>281450.5</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45117.778391203698</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>70000</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44938.614351851851</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>98301.5</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44985.354097222233</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>89100</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45063.792291666658</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45017.004837962973</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>87500</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45169.64203703704</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45000.542685185188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>90000</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66720A0D-E915-4D6C-B7E9-17B6842CE17D}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -696,31 +1290,31 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+      <c r="J1" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>44996.547291666669</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>135000</v>
@@ -728,31 +1322,32 @@
       <c r="I2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
-        <v>16</v>
+      <c r="J2" t="str">
+        <f>_xlfn.TEXTJOIN(", ", TRUE, A2, C2, D2)</f>
+        <v>Senior Data Engineer, Aliso Viejo, CA, United States</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>45097.915243055562</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
       </c>
       <c r="H3">
         <v>35000</v>
@@ -760,176 +1355,182 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
-        <v>23</v>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J21" si="0">_xlfn.TEXTJOIN(", ", TRUE, A3, C3, D3)</f>
+        <v>Data Analyst, Anywhere, Malta</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>45173.250416666669</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>27</v>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Analyst, Reston, VA, United States</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2">
         <v>45156.253321759257</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>31</v>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Cupertino, CA, United States</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2">
         <v>45147.802951388891</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>36</v>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Senior Data Analyst, Rochester, MN, Sudan</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <v>45202.753101851849</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
-        <v>40</v>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Des Moines, IA, United States</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>44949.850462962961</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
-        <v>43</v>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Analyst, Atlanta, GA, United States</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>45001.627175925933</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9">
         <v>115000</v>
@@ -937,60 +1538,62 @@
       <c r="I9" t="b">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
-        <v>47</v>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Analyst, Jacksonville, FL, United States</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>45041.375868055547</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
-        <v>50</v>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Analyst, Dublin, CA, United States</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>45106.587094907409</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11">
         <v>105000</v>
@@ -998,31 +1601,32 @@
       <c r="I11" t="b">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
-        <v>54</v>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Analyst, Charlotte, NC, United States</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>45029.919687499998</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12">
         <v>195000</v>
@@ -1030,31 +1634,32 @@
       <c r="I12" t="b">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
-        <v>57</v>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Sunnyvale, CA, United States</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2">
         <v>45091.502789351849</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13">
         <v>165000</v>
@@ -1062,31 +1667,32 @@
       <c r="I13" t="b">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>61</v>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>Senior Data Scientist, Pasadena, CA, United States</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>45175.543124999997</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14">
         <v>281450.5</v>
@@ -1094,31 +1700,32 @@
       <c r="I14" t="b">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
-        <v>65</v>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Houston, TX, United States</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2">
         <v>45117.778391203698</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15">
         <v>70000</v>
@@ -1126,31 +1733,32 @@
       <c r="I15" t="b">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>70</v>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Johannesburg, South Africa, South Africa</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2">
         <v>44938.614351851851</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16">
         <v>98301.5</v>
@@ -1158,31 +1766,32 @@
       <c r="I16" t="b">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>75</v>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Engineer, Berlin, Germany, Germany</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2">
         <v>44985.354097222233</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17">
         <v>89100</v>
@@ -1190,60 +1799,62 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" t="s">
-        <v>79</v>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Engineer, Amsterdam, Netherlands, Netherlands</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2">
         <v>45063.792291666658</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
-        <v>83</v>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>Business Analyst, Dallas, TX, United States</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>45017.004837962973</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19">
         <v>87500</v>
@@ -1251,60 +1862,62 @@
       <c r="I19" t="b">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
-        <v>86</v>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Broomfield, CO, Sudan</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
         <v>45169.64203703704</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20" t="s">
-        <v>88</v>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>Data Scientist, Anywhere, Sudan</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2">
         <v>45000.542685185188</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21">
         <v>90000</v>
@@ -1312,8 +1925,1483 @@
       <c r="I21" t="b">
         <v>0</v>
       </c>
-      <c r="J21" t="s">
-        <v>92</v>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>Business Analyst, Palo Alto, CA, United States</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468F4981-180C-4B59-ACBA-51E76EAAC562}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44996.547291666669</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>135000</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <f>UPPER(A2)</f>
+        <v>SENIOR DATA ENGINEER</v>
+      </c>
+      <c r="K2" t="str">
+        <f>LOWER(A2)</f>
+        <v>senior data engineer</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45097.915243055562</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>35000</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J21" si="0">UPPER(A3)</f>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K21" si="1">LOWER(A3)</f>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45173.250416666669</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45156.253321759257</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45147.802951388891</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>SENIOR DATA ANALYST</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>senior data analyst</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45202.753101851849</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44949.850462962961</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45001.627175925933</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>115000</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45041.375868055547</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45106.587094907409</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>105000</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ANALYST</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>data analyst</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45029.919687499998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>195000</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45091.502789351849</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>165000</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>SENIOR DATA SCIENTIST</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>senior data scientist</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45175.543124999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>281450.5</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45117.778391203698</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>70000</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44938.614351851851</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>98301.5</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ENGINEER</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>data engineer</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44985.354097222233</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>89100</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA ENGINEER</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>data engineer</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45063.792291666658</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>BUSINESS ANALYST</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>business analyst</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45017.004837962973</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>87500</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45169.64203703704</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>DATA SCIENTIST</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>data scientist</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45000.542685185188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>90000</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>BUSINESS ANALYST</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>business analyst</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5CBE1C-8FD1-4915-9EB1-2C3511AF94AB}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44996.547291666669</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>135000</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <f>TRIM(C2)</f>
+        <v>Aliso Viejo, CA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45097.915243055562</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>35000</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J21" si="0">TRIM(C3)</f>
+        <v>Anywhere</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45173.250416666669</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Reston, VA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45156.253321759257</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Cupertino, CA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45147.802951388891</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Rochester, MN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45202.753101851849</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Des Moines, IA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44949.850462962961</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Atlanta, GA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45001.627175925933</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>115000</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Jacksonville, FL</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45041.375868055547</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Dublin, CA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45106.587094907409</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>105000</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlotte, NC</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45029.919687499998</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>195000</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>Sunnyvale, CA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45091.502789351849</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>165000</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>Pasadena, CA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45175.543124999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>281450.5</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>Houston, TX</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45117.778391203698</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>70000</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>Johannesburg, South Africa</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44938.614351851851</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>98301.5</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>Berlin, Germany</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44985.354097222233</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>89100</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>Amsterdam, Netherlands</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45063.792291666658</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>Dallas, TX</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45017.004837962973</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <v>87500</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>Broomfield, CO</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45169.64203703704</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>Anywhere</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45000.542685185188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>90000</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>Palo Alto, CA</v>
       </c>
     </row>
   </sheetData>

</xml_diff>